<commit_message>
09-11 Chapter OOP course added
</commit_message>
<xml_diff>
--- a/Object-Oriented Programming/OOCourse.xlsx
+++ b/Object-Oriented Programming/OOCourse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3. Михайлов\Develop\PythonTraining\PythonTraining\Object-Oriented Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60C1115-47F2-47CB-B631-91630C81CAC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE061CA-A6FB-4BC8-9115-02238392A010}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10785" xr2:uid="{322C65E7-B1BD-4309-A376-1D5B7C88940C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Chapter 1</t>
   </si>
@@ -82,6 +82,15 @@
   </si>
   <si>
     <t>Стр/пом</t>
+  </si>
+  <si>
+    <t>Ср кол-во стр в день</t>
+  </si>
+  <si>
+    <t>Оцека кол-ва дней до конца</t>
+  </si>
+  <si>
+    <t>Всего помидор</t>
   </si>
 </sst>
 </file>
@@ -511,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{678F2483-BB39-4242-A6CA-6B386A6BC967}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,9 +533,10 @@
     <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>13</v>
       </c>
@@ -545,16 +555,15 @@
       <c r="I1" t="s">
         <v>18</v>
       </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
       <c r="K1" s="2">
-        <f>AVERAGE(G2:G10)</f>
-        <v>28.777777777777779</v>
-      </c>
-      <c r="L1" s="2">
-        <f>(B15-F10)/K1</f>
-        <v>5.8030888030888033</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <f>AVERAGE(G2:G12)</f>
+        <v>31.454545454545453</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -585,8 +594,15 @@
         <f>G2/H2</f>
         <v>9.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="2">
+        <f>(B15-F12)/K1</f>
+        <v>2.4797687861271678</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -617,8 +633,15 @@
         <f t="shared" ref="I3" si="2">G3/H3</f>
         <v>7.333333333333333</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3">
+        <f>SUM(H2:H14)</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -650,7 +673,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -682,7 +705,7 @@
         <v>5.25</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -714,7 +737,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -746,7 +769,7 @@
         <v>4.833333333333333</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -778,7 +801,7 @@
         <v>5.75</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -810,7 +833,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -842,7 +865,7 @@
         <v>6.1111111111111107</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -856,15 +879,25 @@
       <c r="D11" s="1">
         <v>10</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="E11" s="1">
+        <v>282</v>
+      </c>
+      <c r="F11" s="1">
+        <v>335</v>
+      </c>
       <c r="G11" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="H11">
+        <v>12</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" ref="I11:I12" si="4">G11/H11</f>
+        <v>4.416666666666667</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -878,15 +911,25 @@
       <c r="D12" s="1">
         <v>11</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="E12" s="1">
+        <v>336</v>
+      </c>
+      <c r="F12" s="1">
+        <v>370</v>
+      </c>
       <c r="G12" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="H12">
+        <v>6</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="4"/>
+        <v>5.666666666666667</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -908,7 +951,7 @@
       </c>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -930,7 +973,7 @@
       </c>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>448</v>
       </c>

</xml_diff>

<commit_message>
Ch 13 og OOP course
</commit_message>
<xml_diff>
--- a/Object-Oriented Programming/OOCourse.xlsx
+++ b/Object-Oriented Programming/OOCourse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3. Михайлов\Develop\PythonTraining\PythonTraining\Object-Oriented Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE061CA-A6FB-4BC8-9115-02238392A010}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E19417ED-1776-42B5-A116-854DF34EACE2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10785" xr2:uid="{322C65E7-B1BD-4309-A376-1D5B7C88940C}"/>
   </bookViews>
@@ -560,7 +560,7 @@
       </c>
       <c r="K1" s="2">
         <f>AVERAGE(G2:G12)</f>
-        <v>31.454545454545453</v>
+        <v>35.636363636363633</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -599,7 +599,7 @@
       </c>
       <c r="K2" s="2">
         <f>(B15-F12)/K1</f>
-        <v>2.4797687861271678</v>
+        <v>0.8979591836734695</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -638,7 +638,7 @@
       </c>
       <c r="K3">
         <f>SUM(H2:H14)</f>
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -915,18 +915,18 @@
         <v>336</v>
       </c>
       <c r="F12" s="1">
-        <v>370</v>
+        <v>416</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>80</v>
       </c>
       <c r="H12">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I12" s="2">
         <f t="shared" si="4"/>
-        <v>5.666666666666667</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ch 13 OOP course
</commit_message>
<xml_diff>
--- a/Object-Oriented Programming/OOCourse.xlsx
+++ b/Object-Oriented Programming/OOCourse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3. Михайлов\Develop\PythonTraining\PythonTraining\Object-Oriented Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E19417ED-1776-42B5-A116-854DF34EACE2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A227B7-409A-4420-97C6-22B8A5945CFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10785" xr2:uid="{322C65E7-B1BD-4309-A376-1D5B7C88940C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Chapter 1</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Всего помидор</t>
+  </si>
+  <si>
+    <t>Медиана стр/пом</t>
   </si>
 </sst>
 </file>
@@ -522,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{678F2483-BB39-4242-A6CA-6B386A6BC967}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,8 +562,8 @@
         <v>19</v>
       </c>
       <c r="K1" s="2">
-        <f>AVERAGE(G2:G12)</f>
-        <v>35.636363636363633</v>
+        <f>AVERAGE(G2:G13)</f>
+        <v>35.25</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -598,8 +601,8 @@
         <v>20</v>
       </c>
       <c r="K2" s="2">
-        <f>(B15-F12)/K1</f>
-        <v>0.8979591836734695</v>
+        <f>(B15-F13)/K1</f>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -638,7 +641,7 @@
       </c>
       <c r="K3">
         <f>SUM(H2:H14)</f>
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -672,6 +675,13 @@
         <f t="shared" ref="I4:I10" si="3">G4/H4</f>
         <v>2.5</v>
       </c>
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="2">
+        <f>MEDIAN(I2:I13)</f>
+        <v>5.5</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -943,13 +953,23 @@
       <c r="D13" s="1">
         <v>12</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="E13" s="1">
+        <v>417</v>
+      </c>
+      <c r="F13" s="1">
+        <v>448</v>
+      </c>
       <c r="G13" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="2"/>
+        <v>31</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" ref="I13" si="5">G13/H13</f>
+        <v>7.75</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">

</xml_diff>